<commit_message>
Adding DriverScript2 which reads Excelsheet for one case and calls from ActionsKeyword.java
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DF7893-7CE1-4386-83F8-7C811370EA72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD4D6D1-8A52-43B2-9A79-794C9702D8E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Object repository and changes were made to accommodate the OR in the DriverScript_4
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD4D6D1-8A52-43B2-9A79-794C9702D8E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAB417A-7A1C-48CD-B3C1-8C5CB0E3D3E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -116,6 +116,27 @@
   </si>
   <si>
     <t>close_broswer</t>
+  </si>
+  <si>
+    <t>PageObject</t>
+  </si>
+  <si>
+    <t>login_txtBox_empName</t>
+  </si>
+  <si>
+    <t>login_txtBox_empNumber</t>
+  </si>
+  <si>
+    <t>login_txtBox_password</t>
+  </si>
+  <si>
+    <t>login_txtBox_CnfrmPassword</t>
+  </si>
+  <si>
+    <t>login_btn_submit</t>
+  </si>
+  <si>
+    <t>login_div_result</t>
   </si>
 </sst>
 </file>
@@ -463,21 +484,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,10 +510,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -501,11 +526,12 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -515,11 +541,12 @@
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -530,10 +557,13 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -544,10 +574,13 @@
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -558,10 +591,13 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -572,10 +608,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -586,10 +625,13 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -600,10 +642,13 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -613,7 +658,8 @@
       <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Under Maintenance : working on testdata sheet and java files associated to make sure only requred cases run
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAB417A-7A1C-48CD-B3C1-8C5CB0E3D3E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62A2A9E-9BFB-437A-8560-218A8430927D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
+    <sheet name="TestSteps" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -34,9 +35,6 @@
     <t>Action_Keyword</t>
   </si>
   <si>
-    <t>Successfull_login_01</t>
-  </si>
-  <si>
     <t>TS_01</t>
   </si>
   <si>
@@ -137,6 +135,27 @@
   </si>
   <si>
     <t>login_div_result</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Login_01</t>
+  </si>
+  <si>
+    <t>login_01</t>
+  </si>
+  <si>
+    <t>Login_02</t>
+  </si>
+  <si>
+    <t>Successful Registration on entering same password in both the fields</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Error message on entering different values in both the fields</t>
   </si>
 </sst>
 </file>
@@ -483,12 +502,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2D6469-2577-4D38-B0E4-BF7733010CE3}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -510,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -518,149 +587,149 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>